<commit_message>
Enhance domain validation and data input: Remove "Website Name" field, automate niche detection, and enforce price/TAT logic based on domain type.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: c2321058-70e0-4aa3-92ca-d016132b3995
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/b62911d1-db35-4b2e-a422-b493f70d73bd/1ba6fad8-2365-4f12-9813-6b1d980e1dcb.jpg
</commit_message>
<xml_diff>
--- a/client/public/templates/domains-template.xlsx
+++ b/client/public/templates/domains-template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,71 +433,59 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="18" customWidth="1" min="7" max="7"/>
     <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
-    <col width="18" customWidth="1" min="10" max="10"/>
-    <col width="40" customWidth="1" min="11" max="11"/>
+    <col width="40" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Website Name</t>
+          <t>Website URL</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Website URL</t>
+          <t>Domain Rating</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Domain Rating</t>
+          <t>Website Traffic</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Website Traffic</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Niche</t>
+          <t>Guest Post Price</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Niche Edit Price</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Guest Post Price</t>
+          <t>GP TAT (in days)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Niche Edit Price</t>
+          <t>NE TAT (in days)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>GP TAT (in days)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>NE TAT (in days)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Guidelines</t>
         </is>
@@ -506,39 +494,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Example Site</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>example.com</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>75</v>
+      </c>
       <c r="C2" t="n">
-        <v>75</v>
-      </c>
-      <c r="D2" t="n">
         <v>25000</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>SEO</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>guest_post</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>10</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Please provide well-researched content</t>
         </is>
@@ -547,39 +525,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Example Blog</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>blog-example.com</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>68</v>
+      </c>
       <c r="C3" t="n">
-        <v>68</v>
-      </c>
-      <c r="D3" t="n">
         <v>18000</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>niche_edit</t>
         </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>280</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>280</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
         <v>7</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>No branded anchor text</t>
         </is>
@@ -588,43 +556,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Multi Example</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
           <t>multi-example.com</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>72</v>
+      </c>
       <c r="C4" t="n">
-        <v>72</v>
-      </c>
-      <c r="D4" t="n">
         <v>32000</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Technology</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>both</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>400</v>
+      </c>
+      <c r="F4" t="n">
+        <v>320</v>
+      </c>
       <c r="G4" t="n">
-        <v>400</v>
+        <v>14</v>
       </c>
       <c r="H4" t="n">
-        <v>320</v>
-      </c>
-      <c r="I4" t="n">
-        <v>14</v>
-      </c>
-      <c r="J4" t="n">
         <v>7</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Must be related to tech industry</t>
         </is>

</xml_diff>